<commit_message>
9/19/2024 - Admin Mgmt System
</commit_message>
<xml_diff>
--- a/VendorInfo.xlsx
+++ b/VendorInfo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jesus\Desktop\WinFormsApp-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2018DE11-7C1B-47EE-8707-CB34C7FC77DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{198049FB-4059-4AAB-A5A8-01C9D478068D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="690" yWindow="690" windowWidth="26655" windowHeight="11295" xr2:uid="{5F3B18D5-44BA-4945-B1D6-A7140318F147}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Name</t>
   </si>
@@ -84,6 +84,9 @@
   </si>
   <si>
     <t>Paid</t>
+  </si>
+  <si>
+    <t>ID</t>
   </si>
 </sst>
 </file>
@@ -455,67 +458,73 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2656B108-B7AC-4657-9073-B850193AF5D5}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>11</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>12</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>13</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>14</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>